<commit_message>
Added new financial institution from agent extraction
</commit_message>
<xml_diff>
--- a/python/Wave form.xlsx
+++ b/python/Wave form.xlsx
@@ -1195,16 +1195,146 @@
       </c>
     </row>
     <row r="4" customFormat="1" s="18">
-      <c r="B4" s="19" t="n"/>
-      <c r="C4" s="19" t="n"/>
-      <c r="F4" s="20" t="n"/>
-      <c r="G4" s="20" t="n"/>
-      <c r="H4" s="21" t="n"/>
-      <c r="P4" s="22" t="n"/>
-      <c r="S4" s="12" t="n"/>
-      <c r="Z4" s="23" t="n"/>
-      <c r="AA4" s="23" t="n"/>
-      <c r="AB4" s="23" t="n"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>First National Bank</t>
+        </is>
+      </c>
+      <c r="B4" s="19" t="inlineStr">
+        <is>
+          <t>123 Main Street</t>
+        </is>
+      </c>
+      <c r="C4" s="19" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
+      <c r="F4" s="20" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="G4" s="20" t="inlineStr">
+        <is>
+          <t>john.doe@fnb.com</t>
+        </is>
+      </c>
+      <c r="H4" s="21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>67890</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>456789</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="P4" s="22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>AIM123</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S4" s="12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>VAU001</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>MC123</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>9876543210</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>987654321</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>DDA</t>
+        </is>
+      </c>
+      <c r="Z4" s="23" t="inlineStr">
+        <is>
+          <t>RN123456</t>
+        </is>
+      </c>
+      <c r="AA4" s="23" t="inlineStr">
+        <is>
+          <t>654321987</t>
+        </is>
+      </c>
+      <c r="AB4" s="23" t="inlineStr">
+        <is>
+          <t>DDA</t>
+        </is>
+      </c>
     </row>
     <row r="5" customFormat="1" s="18">
       <c r="A5" s="12" t="n"/>

</xml_diff>